<commit_message>
upload and update library
2026.01.26
WR-NPC2
WE-VD
</commit_message>
<xml_diff>
--- a/Git_WE_KiCad_Released_Series_List.xlsx
+++ b/Git_WE_KiCad_Released_Series_List.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A258"/>
+  <dimension ref="A1:A284"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,1790 +450,1972 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>WE-BAL</t>
+          <t>WA-BCMC</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>WCAP-AI3H</t>
+          <t>WA-BCPH</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>WCAP-AIE8</t>
+          <t>WA-MTAB</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>WCAP-AIG5</t>
+          <t>WA-SMCH</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>WCAP-AIG8</t>
+          <t>WE-BAL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>WCAP-AS5H</t>
+          <t>WCAP-AI3H</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>WCAP-ASLI</t>
+          <t>WCAP-AIE8</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>WCAP-ASLL</t>
+          <t>WCAP-AIG5</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>WCAP-ASLU</t>
+          <t>WCAP-AIG8</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>WCAP-ASNP</t>
+          <t>WCAP-AS5H</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>WCAP-AT1H</t>
+          <t>WCAP-ASLI</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>WCAP-ATET</t>
+          <t>WCAP-ASLL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>WCAP-ATG5</t>
+          <t>WCAP-ASLU</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>WCAP-ATG8</t>
+          <t>WCAP-ASNP</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>WCAP-ATLI</t>
+          <t>WCAP-AT1H</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>WCAP-ATLL</t>
+          <t>WCAP-ATET</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>WCAP-ATUL</t>
+          <t>WCAP-ATG5</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>WCAP-CSGP</t>
+          <t>WCAP-ATG8</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>WCAP-CSMH</t>
+          <t>WCAP-ATLI</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>WCAP-CSRF</t>
+          <t>WCAP-ATLL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>WCAP-CSSA</t>
+          <t>WCAP-ATUL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>WCAP-CSST</t>
+          <t>WCAP-CSGP</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>WCAP-FTBE</t>
+          <t>WCAP-CSMH</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>WCAP-FTBP</t>
+          <t>WCAP-CSRF</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>WCAP-FTDB</t>
+          <t>WCAP-CSSA</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>WCAP-FTX2</t>
+          <t>WCAP-CSST</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>WCAP-FTXH</t>
+          <t>WCAP-FTBE</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>WCAP-FTXX</t>
+          <t>WCAP-FTBP</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>WCAP-FTY2</t>
+          <t>WCAP-FTDB</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>WCAP-HSAH</t>
+          <t>WCAP-FTX2</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>WCAP-HSG5</t>
+          <t>WCAP-FTXH</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>WCAP-HTAH</t>
+          <t>WCAP-FTXX</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>WCAP-HTG5</t>
+          <t>WCAP-FTY2</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>WCAP-PHGP</t>
+          <t>WCAP-HSAH</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>WCAP-PHLE</t>
+          <t>WCAP-HSG5</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>WCAP-PHSE</t>
+          <t>WCAP-HTAH</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>WCAP-PSHP</t>
+          <t>WCAP-HTG5</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>WCAP-PSLC</t>
+          <t>WCAP-PHGP</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>WCAP-PSLP</t>
+          <t>WCAP-PHLE</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>WCAP-PT5H</t>
+          <t>WCAP-PHSE</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>WCAP-PTG5</t>
+          <t>WCAP-PSHP</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>WCAP-PTHR</t>
+          <t>WCAP-PSLC</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>WCAP-PTHT</t>
+          <t>WCAP-PSLP</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>WCAP-SISC</t>
+          <t>WCAP-PT5H</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>WCAP-STSC</t>
+          <t>WCAP-PTG5</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>WE-EPLE</t>
+          <t>WCAP-PTHR</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>WR-BHD</t>
+          <t>WCAP-PTHT</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>WR-BTB</t>
+          <t>WCAP-SISC</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>WR-DC</t>
+          <t>WCAP-STSC</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>WR-DSUB</t>
+          <t>WE-EPLE</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>WR-FAST</t>
+          <t>WR-BHD</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>WR-HDMI</t>
+          <t>WR-BTB</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>WR-MJ</t>
+          <t>WR-DC</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>WR-MM</t>
+          <t>WR-DSUB</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>WR-MPC3</t>
+          <t>WR-FAST</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>WR-MPC4</t>
+          <t>WR-HDMI</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>WR-MPC5</t>
+          <t>WR-MJ</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>WR-PHD</t>
+          <t>WR-MM</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>WR-RAST</t>
+          <t>WR-MPC3</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>WR-WTB</t>
+          <t>WR-MPC4</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>WE-SPXO</t>
+          <t>WR-MPC5</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>WE-XTAL</t>
+          <t>WR-NPC2</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>WE-TVSP</t>
+          <t>WR-PHD</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>WE-VE-femtoF</t>
+          <t>WR-RAST</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>WE-VE-ULC</t>
+          <t>WR-WTB</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>WE-VE</t>
+          <t>WE-SPXO</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>WE-VEA</t>
+          <t>WE-XTAL</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>WE-CBA</t>
+          <t>WE-TVSP</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>WE-CBF-HF</t>
+          <t>WE-VE-femtoF</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>WE-CBF</t>
+          <t>WE-VE-ULC</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>WE-CMS</t>
+          <t>WE-VE</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>WE-MLS</t>
+          <t>WE-VEA</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>WE-MPSB</t>
+          <t>WE-CBA</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>WE-PBF</t>
+          <t>WE-CBF-HF</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>WE-PF</t>
+          <t>WE-CBF</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>WE-TMSB</t>
+          <t>WE-CMS</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>WE-UKW</t>
+          <t>WE-MLS</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>WE-WAFB</t>
+          <t>WE-MPSB</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>WE-BPF</t>
+          <t>WE-PBF</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>WE-LPF</t>
+          <t>WE-PF</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>WE-ACHC</t>
+          <t>WE-TMSB</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>WE-ASI</t>
+          <t>WE-UKW</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>WE-CAIR</t>
+          <t>WE-WAFB</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>WE-CCMF</t>
+          <t>WE-BPF</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>WE-CFWI</t>
+          <t>WE-LPF</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>WE-CHSA</t>
+          <t>WE-ACHC</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>WE-CMANC</t>
+          <t>WE-ASI</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>WE-CMB</t>
+          <t>WE-CAIR</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>WE-CMBH</t>
+          <t>WE-CCMF</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>WE-CMBHC</t>
+          <t>WE-CFWI</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>WE-CMBHV</t>
+          <t>WE-CHSA</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>WE-CMBNC</t>
+          <t>WE-CMANC</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>WE-CMBNiZn</t>
+          <t>WE-CMB</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>WE-CMDC</t>
+          <t>WE-CMBH</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>WE-CNSA</t>
+          <t>WE-CMBHC</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>WE-CNSW-HF</t>
+          <t>WE-CMBHV</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>WE-CNSW</t>
+          <t>WE-CMBNC</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>WE-DCT</t>
+          <t>WE-CMBNiZn</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>WE-DD</t>
+          <t>WE-CMDC</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>WE-DPC</t>
+          <t>WE-CNSA</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>WE-DPCHV</t>
+          <t>WE-CNSW-HF</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>WE-EHPI</t>
+          <t>WE-CNSW</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>WE-ExB</t>
+          <t>WE-DCT</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>WE-FAMI</t>
+          <t>WE-DD</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>WE-FC</t>
+          <t>WE-DPC</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>WE-FCLP</t>
+          <t>WE-DPCHV</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>WE-FI</t>
+          <t>WE-EHPI</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>WE-GF</t>
+          <t>WE-ExB</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>WE-GFH</t>
+          <t>WE-FAMI</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>WE-HCC</t>
+          <t>WE-FC</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>WE-HCF</t>
+          <t>WE-FCLP</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>WE-HCFAT</t>
+          <t>WE-FI</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>WE-HCFT</t>
+          <t>WE-GF</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>WE-HCI</t>
+          <t>WE-GFH</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>WE-HCIA</t>
+          <t>WE-HCC</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>WE-HCIT</t>
+          <t>WE-HCF</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>WE-HCM</t>
+          <t>WE-HCFAT</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>WE-HCMD</t>
+          <t>WE-HCFT</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>WE-HEPA</t>
+          <t>WE-HCI</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>WE-HEPC</t>
+          <t>WE-HCIA</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>WE-HIDA</t>
+          <t>WE-HCIT</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>WE-KI</t>
+          <t>WE-HCM</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>WE-KIHC</t>
+          <t>WE-HCMD</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>WE-LF-SMD</t>
+          <t>WE-HEPA</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>WE-LF</t>
+          <t>WE-HEPC</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>WE-LHCA</t>
+          <t>WE-HIDA</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>WE-LHMD</t>
+          <t>WE-KI</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>WE-LHMI</t>
+          <t>WE-KIHC</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>WE-LPCC</t>
+          <t>WE-LF-SMD</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>WE-LQ</t>
+          <t>WE-LF</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>WE-LQFS</t>
+          <t>WE-LHCA</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>WE-LQS</t>
+          <t>WE-LHMD</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>WE-LQSA</t>
+          <t>WE-LHMI</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>WE-LQSH</t>
+          <t>WE-LPCC</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>WE-MAIA</t>
+          <t>WE-LQ</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>WE-MAPI</t>
+          <t>WE-LQFS</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>WE-MCI</t>
+          <t>WE-LQS</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>WE-MCRI</t>
+          <t>WE-LQSA</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>WE-MI</t>
+          <t>WE-LQSH</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>WE-MK</t>
+          <t>WE-MAIA</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>WE-MTCI</t>
+          <t>WE-MAPI</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>WE-MXGA</t>
+          <t>WE-MCI</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>WE-MXGI</t>
+          <t>WE-MCRI</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>WE-PD</t>
+          <t>WE-MI</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>WE-PD2</t>
+          <t>WE-MK</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>WE-PD2A</t>
+          <t>WE-MTCI</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>WE-PD2HV</t>
+          <t>WE-MXGA</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>WE-PD2SA</t>
+          <t>WE-MXGI</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>WE-PD2SR</t>
+          <t>WE-PD</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>WE-PD3</t>
+          <t>WE-PD2</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>WE-PD4</t>
+          <t>WE-PD2A</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>WE-PDA</t>
+          <t>WE-PD2HV</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>WE-PDF</t>
+          <t>WE-PD2SA</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>WE-PDHV</t>
+          <t>WE-PD2SR</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>WE-PMCI</t>
+          <t>WE-PD3</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>WE-PMFI</t>
+          <t>WE-PD4</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>WE-PMI</t>
+          <t>WE-PDA</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>WE-RCIS</t>
+          <t>WE-PDF</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>WE-RCIT</t>
+          <t>WE-PDHV</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>WE-RFH</t>
+          <t>WE-PMCI</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>WE-RFI</t>
+          <t>WE-PMFI</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>WE-SCC</t>
+          <t>WE-PMI</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>WE-SD</t>
+          <t>WE-RCIS</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>WE-SI</t>
+          <t>WE-RCIT</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>WE-SL</t>
+          <t>WE-RFH</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>WE-SL1</t>
+          <t>WE-RFI</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>WE-SL2</t>
+          <t>WE-SCC</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>WE-SL3</t>
+          <t>WE-SD</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>WE-SL5</t>
+          <t>WE-SI</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>WE-SL5HC</t>
+          <t>WE-SL</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>WE-SLM</t>
+          <t>WE-SL1</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>WE-SPC</t>
+          <t>WE-SL2</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>WE-SUKW</t>
+          <t>WE-SL3</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>WE-TCI</t>
+          <t>WE-SL5</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>WE-TDC</t>
+          <t>WE-SL5HC</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>WE-TDCHV</t>
+          <t>WE-SLM</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>WE-TFC</t>
+          <t>WE-SPC</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>WE-TI</t>
+          <t>WE-SUKW</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>WE-TIHV</t>
+          <t>WE-TCI</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>WE-TIS</t>
+          <t>WE-TDC</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>WE-TORPFC</t>
+          <t>WE-TDCHV</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>WE-TPB</t>
+          <t>WE-TFC</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>WE-TPBHV</t>
+          <t>WE-TI</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>WE-TPC</t>
+          <t>WE-TIHV</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>WE-UCF</t>
+          <t>WE-TIS</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>WE-WPCC</t>
+          <t>WE-TORPFC</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>WE-XHMA</t>
+          <t>WE-TPB</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>WE-XHMI</t>
+          <t>WE-TPBHV</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>WL-SMDC</t>
+          <t>WE-TPC</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>MagIC-FDSM</t>
+          <t>WE-UCF</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>MagIC-FIMM</t>
+          <t>WE-WPCC</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>MagIC-LDHM</t>
+          <t>WE-XHMA</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>MagIC-VDRM</t>
+          <t>WE-XHMI</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>MagIC-VISM</t>
+          <t>WL-SMDC</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>WPME-CDIP</t>
+          <t>MagIC-FDSM</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>WPME-CDIS</t>
+          <t>MagIC-FIMM</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>WPME-FISM</t>
+          <t>MagIC-LDHM</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>WPME-VDLM</t>
+          <t>MagIC-VDRM</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>WPME-VDMM</t>
+          <t>MagIC-VISM</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>WL-OCTR</t>
+          <t>WPME-CDIP</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>WRIS-KSKE</t>
+          <t>WPME-CDIS</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>WRIS-KWKB</t>
+          <t>WPME-FISM</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>WRIS-KWKH</t>
+          <t>WPME-VDLM</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>WRIS-PSMB</t>
+          <t>WPME-VDMM</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>WRIS-PSMC</t>
+          <t>WL-OCTR</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>WRIS-RSKS</t>
+          <t>WIRL</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>WE-RCDS</t>
+          <t>WP-BUCF</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>WE-SECF</t>
+          <t>WP-BUFU</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>WE-SHC</t>
+          <t>WP-BUTR</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>WE-SMGS</t>
+          <t>WP-PFEFUA</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>WS-MITV</t>
+          <t>WP-PFICFA</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>WS-ROTV</t>
+          <t>WP-PFIFUA</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>WS-TOTV</t>
+          <t>WP-PLUG</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>WE-AGDT</t>
+          <t>WP-RAFE</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>WE-BMS</t>
+          <t>WP-RAFU</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>WE-CST</t>
+          <t>WP-RATR</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>WE-CSTLF</t>
+          <t>WP-SHFU</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>WE-FB</t>
+          <t>WP-SMBU</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>WE-FB3751</t>
+          <t>WP-SMRA</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>WE-FLEX+</t>
+          <t>WP-SMRT</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>WE-FLEX</t>
+          <t>WP-SMSH</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>WE-FLEXHV</t>
+          <t>WP-TGCF</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>WE-FLYLT</t>
+          <t>WP-TGTR</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>WE-FLYTI</t>
+          <t>WP-THRBU</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>WE-GDT</t>
+          <t>WP-THRSH</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>WE-GDTI</t>
+          <t>WRIS-KSKE</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>WE-IBTI</t>
+          <t>WRIS-KWKB</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>WE-LAN</t>
+          <t>WRIS-KWKH</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>WE-LAN10G</t>
+          <t>WRIS-PSMB</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>WE-LANAQ</t>
+          <t>WRIS-PSMC</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>WE-LANMX</t>
+          <t>WRIS-RSKS</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>WE-LLCR</t>
+          <t>WE-RCDS</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>WE-OLEE</t>
+          <t>WE-SCFA</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>WE-OLEFD</t>
+          <t>WE-SECF</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>WE-OLLT</t>
+          <t>WE-SHC</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>WE-OLPI</t>
+          <t>WE-SMGS</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>WE-OLRM</t>
+          <t>WS-MITV</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>WE-OLSTM</t>
+          <t>WS-ROTV</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>WE-OLTI</t>
+          <t>WS-TOTV</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>WE-PFC</t>
+          <t>WE-AGDT</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>WE-PLC</t>
+          <t>WE-BMS</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>WE-PLN</t>
+          <t>WE-CST</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>WE-PoE++</t>
+          <t>WE-CSTLF</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>WE-PoE+</t>
+          <t>WE-FB</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>WE-PoE</t>
+          <t>WE-FB3751</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>WE-PoEH</t>
+          <t>WE-FLEX+</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>WE-PPTI</t>
+          <t>WE-FLEX</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>WE-PPTM</t>
+          <t>WE-FLEXHV</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>WE-PSPA</t>
+          <t>WE-FLYLT</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>WE-RJ45LAN</t>
+          <t>WE-FLYTI</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>WE-SPE</t>
+          <t>WE-GDT</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>WE-STST</t>
+          <t>WE-GDTI</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>WE-UNIT</t>
+          <t>WE-IBTI</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>WE-UOST</t>
+          <t>WE-LAN</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>WE-VD</t>
+          <t>WE-LAN10G</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
+        <is>
+          <t>WE-LANAQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>WE-LANMX</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>WE-LLCR</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>WE-OLEE</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>WE-OLEFD</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>WE-OLLT</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>WE-OLPI</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>WE-OLRM</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>WE-OLSTM</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>WE-OLTI</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>WE-PFC</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>WE-PLC</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>WE-PLN</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>WE-PoE++</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>WE-PoE+</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>WE-PoE</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>WE-PoEH</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>WE-PPTI</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>WE-PPTM</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>WE-PSPA</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>WE-RJ45LAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>WE-SPE</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>WE-STST</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>WE-UNIT</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>WE-UOST</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>WE-VD</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
         <is>
           <t>WE-VS</t>
         </is>

</xml_diff>